<commit_message>
remove generic person attributes from cookiecutter setup
</commit_message>
<xml_diff>
--- a/project/excel/test_case_schema.xlsx
+++ b/project/excel/test_case_schema.xlsx
@@ -7,9 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="TestCase" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="TestCaseCollection" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="TestCase" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="TestCaseCollection" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -415,98 +414,19 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>primary_email</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>birth_date</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>age_in_years</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>vital_status</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"ALIVE,DEAD,UNKNOWN"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
schema for current semantic smoke test input
</commit_message>
<xml_diff>
--- a/project/excel/test_case_schema.xlsx
+++ b/project/excel/test_case_schema.xlsx
@@ -8,7 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="TestCase" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="TestCaseCollection" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="SemanticSmokeTestCase" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Input" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="SemanticSmokeTestInput" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Output" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="SemanticSmokeTestOutput" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Precondition" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="TestSuite" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -414,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,6 +444,21 @@
           <t>description</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>inputs</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>outputs</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>preconditions</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -445,6 +466,216 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>inputs</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>outputs</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>preconditions</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>must_pass_date</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>must_pass_environment</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>query</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>string_entry</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>direction</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>answer_informal_concept</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>expected_result</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>curie</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>top_level</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>node</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>notes</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"DEV,CI,TEST,PROD"</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"increased,decreased"</formula1>
+    </dataValidation>
+    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"include_good,exclude_bad"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>